<commit_message>
hot fix report file: change color
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR002_FS.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR002_FS.xlsx
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,14 +148,28 @@
       <charset val="128"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +188,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="46">
     <border>
@@ -723,54 +743,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
@@ -783,69 +789,12 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="40" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="41" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="35" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="39" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -870,24 +819,9 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="28" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -921,36 +855,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="28" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="29" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="31" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="31" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="30" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -969,42 +873,160 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="45" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="32" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="34" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="36" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="28" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="8" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="37" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="43" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="29" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="30" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="30" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="28" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="33" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent5" xfId="3" builtinId="46"/>
+    <cellStyle name="60% - Accent5" xfId="4" builtinId="48"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="標準 10" xfId="2"/>
     <cellStyle name="標準 3" xfId="1"/>
@@ -1321,769 +1343,768 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="Q1" zoomScale="280" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="280" workbookViewId="0">
-      <selection activeCell="AL5" sqref="AL5:AM7"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="205" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="205" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="9.75" customHeight="1"/>
   <cols>
-    <col min="1" max="57" width="2.42578125" style="2" customWidth="1"/>
-    <col min="58" max="91" width="2.7109375" style="2" customWidth="1"/>
-    <col min="92" max="16384" width="3.140625" style="2"/>
+    <col min="1" max="57" width="2.42578125" style="1" customWidth="1"/>
+    <col min="58" max="91" width="2.7109375" style="1" customWidth="1"/>
+    <col min="92" max="16384" width="3.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:86" ht="9.9499999999999993" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="40" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="BG1" s="17"/>
-      <c r="BH1" s="15"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="14"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="14"/>
-      <c r="BM1" s="9"/>
-      <c r="BN1" s="11"/>
-      <c r="BO1" s="9"/>
-      <c r="BP1" s="11"/>
-      <c r="BQ1" s="9"/>
-      <c r="BR1" s="11"/>
-      <c r="BS1" s="9"/>
-      <c r="BT1" s="11"/>
-      <c r="BU1" s="9"/>
-      <c r="BV1" s="11"/>
-      <c r="BW1" s="9"/>
-      <c r="BX1" s="11"/>
-      <c r="BY1" s="9"/>
-      <c r="BZ1" s="11"/>
-      <c r="CA1" s="19"/>
-      <c r="CB1" s="20"/>
-      <c r="CC1" s="9"/>
-      <c r="CD1" s="11"/>
-      <c r="CE1" s="21"/>
-      <c r="CF1" s="20"/>
-      <c r="CG1" s="9"/>
-      <c r="CH1" s="10"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="10"/>
+      <c r="BI1" s="6"/>
+      <c r="BJ1" s="8"/>
+      <c r="BK1" s="6"/>
+      <c r="BL1" s="8"/>
+      <c r="BM1" s="6"/>
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="6"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="6"/>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="6"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="6"/>
+      <c r="BV1" s="8"/>
+      <c r="BW1" s="6"/>
+      <c r="BX1" s="8"/>
+      <c r="BY1" s="6"/>
+      <c r="BZ1" s="8"/>
+      <c r="CA1" s="6"/>
+      <c r="CB1" s="8"/>
+      <c r="CC1" s="6"/>
+      <c r="CD1" s="8"/>
+      <c r="CE1" s="7"/>
+      <c r="CF1" s="8"/>
+      <c r="CG1" s="6"/>
+      <c r="CH1" s="7"/>
     </row>
     <row r="2" spans="1:86" ht="9.9499999999999993" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="BG2" s="18"/>
-      <c r="BH2" s="16"/>
-      <c r="BI2" s="13"/>
-      <c r="BJ2" s="14"/>
-      <c r="BK2" s="13"/>
-      <c r="BL2" s="14"/>
-      <c r="BM2" s="9"/>
-      <c r="BN2" s="11"/>
-      <c r="BO2" s="9"/>
-      <c r="BP2" s="11"/>
-      <c r="BQ2" s="9"/>
-      <c r="BR2" s="11"/>
-      <c r="BS2" s="9"/>
-      <c r="BT2" s="11"/>
-      <c r="BU2" s="9"/>
-      <c r="BV2" s="11"/>
-      <c r="BW2" s="9"/>
-      <c r="BX2" s="11"/>
-      <c r="BY2" s="9"/>
-      <c r="BZ2" s="11"/>
-      <c r="CA2" s="19"/>
-      <c r="CB2" s="20"/>
-      <c r="CC2" s="9"/>
-      <c r="CD2" s="11"/>
-      <c r="CE2" s="21"/>
-      <c r="CF2" s="20"/>
-      <c r="CG2" s="9"/>
-      <c r="CH2" s="10"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="BG2" s="13"/>
+      <c r="BH2" s="11"/>
+      <c r="BI2" s="6"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="6"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="6"/>
+      <c r="BN2" s="8"/>
+      <c r="BO2" s="6"/>
+      <c r="BP2" s="8"/>
+      <c r="BQ2" s="6"/>
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="6"/>
+      <c r="BT2" s="8"/>
+      <c r="BU2" s="6"/>
+      <c r="BV2" s="8"/>
+      <c r="BW2" s="6"/>
+      <c r="BX2" s="8"/>
+      <c r="BY2" s="6"/>
+      <c r="BZ2" s="8"/>
+      <c r="CA2" s="6"/>
+      <c r="CB2" s="8"/>
+      <c r="CC2" s="6"/>
+      <c r="CD2" s="8"/>
+      <c r="CE2" s="7"/>
+      <c r="CF2" s="8"/>
+      <c r="CG2" s="6"/>
+      <c r="CH2" s="7"/>
     </row>
     <row r="3" spans="1:86" ht="9.75" customHeight="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:86" ht="9.9499999999999993" customHeight="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="48" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="51"/>
-      <c r="W4" s="50"/>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="50"/>
-      <c r="Z4" s="53"/>
-      <c r="AA4" s="50"/>
-      <c r="AB4" s="53"/>
-      <c r="AC4" s="50"/>
-      <c r="AD4" s="53"/>
-      <c r="AE4" s="50"/>
-      <c r="AF4" s="53"/>
-      <c r="AG4" s="50"/>
-      <c r="AH4" s="53"/>
-      <c r="AI4" s="5"/>
-      <c r="AJ4" s="75"/>
-      <c r="AK4" s="75"/>
-      <c r="AL4" s="75"/>
-      <c r="AM4" s="75"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="4"/>
-      <c r="AR4" s="4"/>
-      <c r="AS4" s="4"/>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="6"/>
-      <c r="AW4" s="6"/>
-      <c r="AX4" s="6"/>
-      <c r="AY4" s="6"/>
-      <c r="AZ4" s="6"/>
-      <c r="BA4" s="6"/>
-      <c r="BB4" s="6"/>
-      <c r="BC4" s="6"/>
-      <c r="BD4" s="75"/>
-      <c r="BE4" s="75"/>
-      <c r="BG4" s="17"/>
-      <c r="BH4" s="15"/>
-      <c r="BI4" s="13"/>
-      <c r="BJ4" s="14"/>
-      <c r="BK4" s="13"/>
-      <c r="BL4" s="14"/>
-      <c r="BM4" s="9"/>
-      <c r="BN4" s="11"/>
-      <c r="BO4" s="9"/>
-      <c r="BP4" s="11"/>
-      <c r="BQ4" s="9"/>
-      <c r="BR4" s="11"/>
-      <c r="BS4" s="9"/>
-      <c r="BT4" s="11"/>
-      <c r="BU4" s="9"/>
-      <c r="BV4" s="11"/>
-      <c r="BW4" s="9"/>
-      <c r="BX4" s="11"/>
-      <c r="BY4" s="9"/>
-      <c r="BZ4" s="11"/>
-      <c r="CA4" s="19"/>
-      <c r="CB4" s="20"/>
-      <c r="CC4" s="9"/>
-      <c r="CD4" s="11"/>
-      <c r="CE4" s="21"/>
-      <c r="CF4" s="20"/>
-      <c r="CG4" s="9"/>
-      <c r="CH4" s="10"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="53"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="53"/>
+      <c r="X4" s="54"/>
+      <c r="Y4" s="53"/>
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="53"/>
+      <c r="AB4" s="55"/>
+      <c r="AC4" s="53"/>
+      <c r="AD4" s="55"/>
+      <c r="AE4" s="53"/>
+      <c r="AF4" s="55"/>
+      <c r="AG4" s="53"/>
+      <c r="AH4" s="55"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="36"/>
+      <c r="AK4" s="36"/>
+      <c r="AL4" s="36"/>
+      <c r="AM4" s="36"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="5"/>
+      <c r="AU4" s="5"/>
+      <c r="AV4" s="5"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="5"/>
+      <c r="AY4" s="5"/>
+      <c r="AZ4" s="5"/>
+      <c r="BA4" s="5"/>
+      <c r="BB4" s="5"/>
+      <c r="BC4" s="5"/>
+      <c r="BD4" s="36"/>
+      <c r="BE4" s="36"/>
+      <c r="BG4" s="42"/>
+      <c r="BH4" s="44"/>
+      <c r="BI4" s="46"/>
+      <c r="BJ4" s="47"/>
+      <c r="BK4" s="46"/>
+      <c r="BL4" s="47"/>
+      <c r="BM4" s="46"/>
+      <c r="BN4" s="47"/>
+      <c r="BO4" s="46"/>
+      <c r="BP4" s="47"/>
+      <c r="BQ4" s="46"/>
+      <c r="BR4" s="47"/>
+      <c r="BS4" s="46"/>
+      <c r="BT4" s="47"/>
+      <c r="BU4" s="46"/>
+      <c r="BV4" s="47"/>
+      <c r="BW4" s="46"/>
+      <c r="BX4" s="47"/>
+      <c r="BY4" s="46"/>
+      <c r="BZ4" s="47"/>
+      <c r="CA4" s="46"/>
+      <c r="CB4" s="47"/>
+      <c r="CC4" s="46"/>
+      <c r="CD4" s="47"/>
+      <c r="CE4" s="48"/>
+      <c r="CF4" s="47"/>
+      <c r="CG4" s="46"/>
+      <c r="CH4" s="48"/>
     </row>
     <row r="5" spans="1:86" ht="9.9499999999999993" customHeight="1">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="50" t="s">
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="51"/>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="53"/>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="53"/>
-      <c r="AC5" s="50"/>
-      <c r="AD5" s="53"/>
-      <c r="AE5" s="50"/>
-      <c r="AF5" s="53"/>
-      <c r="AG5" s="50"/>
-      <c r="AH5" s="53"/>
-      <c r="AI5" s="5"/>
-      <c r="AJ5" s="5"/>
-      <c r="AK5" s="5"/>
-      <c r="AL5" s="75"/>
-      <c r="AM5" s="75"/>
-      <c r="AN5" s="4"/>
-      <c r="AO5" s="4"/>
-      <c r="AP5" s="4"/>
-      <c r="AQ5" s="4"/>
-      <c r="AR5" s="4"/>
-      <c r="AS5" s="4"/>
-      <c r="AT5" s="4"/>
-      <c r="AU5" s="4"/>
-      <c r="AV5" s="6"/>
-      <c r="AW5" s="6"/>
-      <c r="AX5" s="6"/>
-      <c r="AY5" s="6"/>
-      <c r="AZ5" s="6"/>
-      <c r="BA5" s="6"/>
-      <c r="BB5" s="6"/>
-      <c r="BC5" s="6"/>
-      <c r="BD5" s="75"/>
-      <c r="BE5" s="75"/>
-      <c r="BG5" s="18"/>
-      <c r="BH5" s="16"/>
-      <c r="BI5" s="13"/>
-      <c r="BJ5" s="14"/>
-      <c r="BK5" s="13"/>
-      <c r="BL5" s="14"/>
-      <c r="BM5" s="9"/>
-      <c r="BN5" s="11"/>
-      <c r="BO5" s="9"/>
-      <c r="BP5" s="11"/>
-      <c r="BQ5" s="9"/>
-      <c r="BR5" s="11"/>
-      <c r="BS5" s="9"/>
-      <c r="BT5" s="11"/>
-      <c r="BU5" s="9"/>
-      <c r="BV5" s="11"/>
-      <c r="BW5" s="9"/>
-      <c r="BX5" s="11"/>
-      <c r="BY5" s="9"/>
-      <c r="BZ5" s="11"/>
-      <c r="CA5" s="19"/>
-      <c r="CB5" s="20"/>
-      <c r="CC5" s="9"/>
-      <c r="CD5" s="11"/>
-      <c r="CE5" s="21"/>
-      <c r="CF5" s="20"/>
-      <c r="CG5" s="9"/>
-      <c r="CH5" s="10"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="54"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="53"/>
+      <c r="Z5" s="55"/>
+      <c r="AA5" s="53"/>
+      <c r="AB5" s="55"/>
+      <c r="AC5" s="53"/>
+      <c r="AD5" s="55"/>
+      <c r="AE5" s="53"/>
+      <c r="AF5" s="55"/>
+      <c r="AG5" s="53"/>
+      <c r="AH5" s="55"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="36"/>
+      <c r="AM5" s="36"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+      <c r="AY5" s="5"/>
+      <c r="AZ5" s="5"/>
+      <c r="BA5" s="5"/>
+      <c r="BB5" s="5"/>
+      <c r="BC5" s="5"/>
+      <c r="BD5" s="36"/>
+      <c r="BE5" s="36"/>
+      <c r="BG5" s="43"/>
+      <c r="BH5" s="45"/>
+      <c r="BI5" s="46"/>
+      <c r="BJ5" s="47"/>
+      <c r="BK5" s="46"/>
+      <c r="BL5" s="47"/>
+      <c r="BM5" s="46"/>
+      <c r="BN5" s="47"/>
+      <c r="BO5" s="46"/>
+      <c r="BP5" s="47"/>
+      <c r="BQ5" s="46"/>
+      <c r="BR5" s="47"/>
+      <c r="BS5" s="46"/>
+      <c r="BT5" s="47"/>
+      <c r="BU5" s="46"/>
+      <c r="BV5" s="47"/>
+      <c r="BW5" s="46"/>
+      <c r="BX5" s="47"/>
+      <c r="BY5" s="46"/>
+      <c r="BZ5" s="47"/>
+      <c r="CA5" s="46"/>
+      <c r="CB5" s="47"/>
+      <c r="CC5" s="46"/>
+      <c r="CD5" s="47"/>
+      <c r="CE5" s="48"/>
+      <c r="CF5" s="47"/>
+      <c r="CG5" s="46"/>
+      <c r="CH5" s="48"/>
     </row>
     <row r="6" spans="1:86" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="47"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="22"/>
-      <c r="X6" s="47"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="23"/>
-      <c r="AG6" s="22"/>
-      <c r="AH6" s="23"/>
-      <c r="AI6" s="5"/>
-      <c r="AJ6" s="5"/>
-      <c r="AK6" s="5"/>
-      <c r="AL6" s="75"/>
-      <c r="AM6" s="75"/>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="4"/>
-      <c r="AP6" s="4"/>
-      <c r="AQ6" s="4"/>
-      <c r="AR6" s="4"/>
-      <c r="AS6" s="4"/>
-      <c r="AT6" s="4"/>
-      <c r="AU6" s="4"/>
-      <c r="AV6" s="6"/>
-      <c r="AW6" s="6"/>
-      <c r="AX6" s="6"/>
-      <c r="AY6" s="6"/>
-      <c r="AZ6" s="6"/>
-      <c r="BA6" s="6"/>
-      <c r="BB6" s="6"/>
-      <c r="BC6" s="6"/>
-      <c r="BD6" s="75"/>
-      <c r="BE6" s="75"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="14"/>
+      <c r="AH6" s="15"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="36"/>
+      <c r="AM6" s="36"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="5"/>
+      <c r="AU6" s="5"/>
+      <c r="AV6" s="5"/>
+      <c r="AW6" s="5"/>
+      <c r="AX6" s="5"/>
+      <c r="AY6" s="5"/>
+      <c r="AZ6" s="5"/>
+      <c r="BA6" s="5"/>
+      <c r="BB6" s="5"/>
+      <c r="BC6" s="5"/>
+      <c r="BD6" s="36"/>
+      <c r="BE6" s="36"/>
     </row>
     <row r="7" spans="1:86" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="47"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="22"/>
-      <c r="X7" s="47"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="22"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="22"/>
-      <c r="AF7" s="23"/>
-      <c r="AG7" s="22"/>
-      <c r="AH7" s="23"/>
-      <c r="AI7" s="5"/>
-      <c r="AJ7" s="91"/>
-      <c r="AK7" s="91"/>
-      <c r="AL7" s="75"/>
-      <c r="AM7" s="75"/>
-      <c r="AN7" s="4"/>
-      <c r="AO7" s="4"/>
-      <c r="AP7" s="4"/>
-      <c r="AQ7" s="4"/>
-      <c r="AR7" s="4"/>
-      <c r="AS7" s="4"/>
-      <c r="AT7" s="4"/>
-      <c r="AU7" s="4"/>
-      <c r="AV7" s="6"/>
-      <c r="AW7" s="6"/>
-      <c r="AX7" s="6"/>
-      <c r="AY7" s="6"/>
-      <c r="AZ7" s="6"/>
-      <c r="BA7" s="6"/>
-      <c r="BB7" s="6"/>
-      <c r="BC7" s="6"/>
-      <c r="BD7" s="75"/>
-      <c r="BE7" s="75"/>
-      <c r="BG7" s="62" t="s">
+      <c r="A7" s="56"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="14"/>
+      <c r="AH7" s="15"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="36"/>
+      <c r="AK7" s="36"/>
+      <c r="AL7" s="36"/>
+      <c r="AM7" s="36"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="5"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="5"/>
+      <c r="AT7" s="5"/>
+      <c r="AU7" s="5"/>
+      <c r="AV7" s="5"/>
+      <c r="AW7" s="5"/>
+      <c r="AX7" s="5"/>
+      <c r="AY7" s="5"/>
+      <c r="AZ7" s="5"/>
+      <c r="BA7" s="5"/>
+      <c r="BB7" s="5"/>
+      <c r="BC7" s="5"/>
+      <c r="BD7" s="36"/>
+      <c r="BE7" s="36"/>
+      <c r="BG7" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="BH7" s="63"/>
-      <c r="BI7" s="64"/>
-      <c r="BJ7" s="64"/>
-      <c r="BK7" s="64"/>
-      <c r="BL7" s="64"/>
-      <c r="BM7" s="64"/>
-      <c r="BN7" s="62" t="s">
+      <c r="BH7" s="34"/>
+      <c r="BI7" s="35"/>
+      <c r="BJ7" s="35"/>
+      <c r="BK7" s="35"/>
+      <c r="BL7" s="35"/>
+      <c r="BM7" s="35"/>
+      <c r="BN7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="BO7" s="63"/>
-      <c r="BP7" s="64"/>
-      <c r="BQ7" s="64"/>
-      <c r="BR7" s="64"/>
-      <c r="BS7" s="64"/>
-      <c r="BT7" s="64"/>
-      <c r="BU7" s="64"/>
-      <c r="BV7" s="64"/>
-      <c r="BW7" s="64"/>
-      <c r="BX7" s="64"/>
-      <c r="BY7" s="64"/>
-      <c r="BZ7" s="64"/>
-      <c r="CA7" s="64"/>
-      <c r="CB7" s="64"/>
-      <c r="CC7" s="64"/>
-      <c r="CD7" s="64"/>
-      <c r="CE7" s="64"/>
-      <c r="CF7" s="64"/>
-      <c r="CG7" s="64"/>
-      <c r="CH7" s="64"/>
+      <c r="BO7" s="34"/>
+      <c r="BP7" s="35"/>
+      <c r="BQ7" s="35"/>
+      <c r="BR7" s="35"/>
+      <c r="BS7" s="35"/>
+      <c r="BT7" s="35"/>
+      <c r="BU7" s="35"/>
+      <c r="BV7" s="35"/>
+      <c r="BW7" s="35"/>
+      <c r="BX7" s="35"/>
+      <c r="BY7" s="35"/>
+      <c r="BZ7" s="35"/>
+      <c r="CA7" s="35"/>
+      <c r="CB7" s="35"/>
+      <c r="CC7" s="35"/>
+      <c r="CD7" s="35"/>
+      <c r="CE7" s="35"/>
+      <c r="CF7" s="35"/>
+      <c r="CG7" s="35"/>
+      <c r="CH7" s="35"/>
     </row>
     <row r="8" spans="1:86" ht="9.75" customHeight="1" thickBot="1">
-      <c r="U8" s="1"/>
-      <c r="V8" s="43"/>
-      <c r="W8" s="44"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="46"/>
-      <c r="Z8" s="46"/>
-      <c r="AA8" s="76"/>
-      <c r="AB8" s="77"/>
-      <c r="AC8" s="46"/>
-      <c r="AD8" s="46"/>
-      <c r="AE8" s="46"/>
-      <c r="AF8" s="76"/>
-      <c r="AG8" s="77"/>
-      <c r="AH8" s="77"/>
-      <c r="AI8" s="46"/>
-      <c r="AJ8" s="46"/>
-      <c r="AK8" s="46"/>
-      <c r="AL8" s="78"/>
-      <c r="AM8" s="79"/>
-      <c r="AN8" s="79"/>
-      <c r="AO8" s="79"/>
-      <c r="AP8" s="79"/>
-      <c r="AQ8" s="79"/>
-      <c r="AR8" s="79"/>
-      <c r="AS8" s="79"/>
-      <c r="AT8" s="79"/>
-      <c r="AU8" s="79"/>
-      <c r="AV8" s="79"/>
-      <c r="AW8" s="79"/>
-      <c r="AX8" s="79"/>
-      <c r="AY8" s="79"/>
-      <c r="AZ8" s="79"/>
-      <c r="BA8" s="79"/>
-      <c r="BB8" s="79"/>
-      <c r="BC8" s="79"/>
-      <c r="BD8" s="80"/>
-      <c r="BE8" s="80"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="37"/>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="37"/>
+      <c r="AG8" s="38"/>
+      <c r="AH8" s="38"/>
+      <c r="AI8" s="22"/>
+      <c r="AJ8" s="22"/>
+      <c r="AK8" s="22"/>
+      <c r="AL8" s="39"/>
+      <c r="AM8" s="40"/>
+      <c r="AN8" s="40"/>
+      <c r="AO8" s="40"/>
+      <c r="AP8" s="40"/>
+      <c r="AQ8" s="40"/>
+      <c r="AR8" s="40"/>
+      <c r="AS8" s="40"/>
+      <c r="AT8" s="40"/>
+      <c r="AU8" s="40"/>
+      <c r="AV8" s="40"/>
+      <c r="AW8" s="40"/>
+      <c r="AX8" s="40"/>
+      <c r="AY8" s="40"/>
+      <c r="AZ8" s="40"/>
+      <c r="BA8" s="40"/>
+      <c r="BB8" s="40"/>
+      <c r="BC8" s="40"/>
+      <c r="BD8" s="41"/>
+      <c r="BE8" s="41"/>
     </row>
     <row r="9" spans="1:86" ht="12.2" customHeight="1" thickBot="1">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="31"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="31"/>
-      <c r="AA9" s="30"/>
-      <c r="AB9" s="81"/>
-      <c r="AD9" s="24" t="s">
+      <c r="D9" s="61"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="63"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="64"/>
+      <c r="AD9" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AE9" s="26" t="s">
+      <c r="AE9" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="AF9" s="83" t="s">
+      <c r="AF9" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="AG9" s="83"/>
-      <c r="AH9" s="30"/>
-      <c r="AI9" s="31"/>
-      <c r="AJ9" s="30"/>
-      <c r="AK9" s="31"/>
-      <c r="AL9" s="30"/>
-      <c r="AM9" s="31"/>
-      <c r="AN9" s="30"/>
-      <c r="AO9" s="31"/>
-      <c r="AP9" s="30"/>
-      <c r="AQ9" s="31"/>
-      <c r="AR9" s="30"/>
-      <c r="AS9" s="31"/>
-      <c r="AT9" s="30"/>
-      <c r="AU9" s="31"/>
-      <c r="AV9" s="30"/>
-      <c r="AW9" s="31"/>
-      <c r="AX9" s="30"/>
-      <c r="AY9" s="31"/>
-      <c r="AZ9" s="30"/>
-      <c r="BA9" s="31"/>
-      <c r="BB9" s="30"/>
-      <c r="BC9" s="31"/>
-      <c r="BD9" s="83"/>
-      <c r="BE9" s="84"/>
-      <c r="BG9" s="62" t="s">
+      <c r="AG9" s="65"/>
+      <c r="AH9" s="62"/>
+      <c r="AI9" s="63"/>
+      <c r="AJ9" s="62"/>
+      <c r="AK9" s="63"/>
+      <c r="AL9" s="62"/>
+      <c r="AM9" s="63"/>
+      <c r="AN9" s="62"/>
+      <c r="AO9" s="63"/>
+      <c r="AP9" s="62"/>
+      <c r="AQ9" s="63"/>
+      <c r="AR9" s="62"/>
+      <c r="AS9" s="63"/>
+      <c r="AT9" s="62"/>
+      <c r="AU9" s="63"/>
+      <c r="AV9" s="62"/>
+      <c r="AW9" s="63"/>
+      <c r="AX9" s="62"/>
+      <c r="AY9" s="63"/>
+      <c r="AZ9" s="62"/>
+      <c r="BA9" s="63"/>
+      <c r="BB9" s="62"/>
+      <c r="BC9" s="63"/>
+      <c r="BD9" s="65"/>
+      <c r="BE9" s="66"/>
+      <c r="BG9" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="BH9" s="63"/>
-      <c r="BI9" s="64"/>
-      <c r="BJ9" s="64"/>
-      <c r="BK9" s="64"/>
-      <c r="BL9" s="62" t="s">
+      <c r="BH9" s="34"/>
+      <c r="BI9" s="35"/>
+      <c r="BJ9" s="35"/>
+      <c r="BK9" s="35"/>
+      <c r="BL9" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="BM9" s="63"/>
-      <c r="BN9" s="64"/>
-      <c r="BO9" s="64"/>
-      <c r="BP9" s="64"/>
-      <c r="BQ9" s="62" t="s">
+      <c r="BM9" s="34"/>
+      <c r="BN9" s="35"/>
+      <c r="BO9" s="35"/>
+      <c r="BP9" s="35"/>
+      <c r="BQ9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="BR9" s="63"/>
-      <c r="BS9" s="63"/>
-      <c r="BT9" s="64"/>
-      <c r="BU9" s="64"/>
-      <c r="BV9" s="64"/>
-      <c r="BW9" s="62" t="s">
+      <c r="BR9" s="34"/>
+      <c r="BS9" s="34"/>
+      <c r="BT9" s="35"/>
+      <c r="BU9" s="35"/>
+      <c r="BV9" s="35"/>
+      <c r="BW9" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="BX9" s="63"/>
-      <c r="BY9" s="63"/>
-      <c r="BZ9" s="63"/>
-      <c r="CA9" s="63"/>
-      <c r="CB9" s="63"/>
-      <c r="CC9" s="63"/>
-      <c r="CD9" s="63"/>
-      <c r="CE9" s="63"/>
-      <c r="CF9" s="63"/>
-      <c r="CG9" s="64"/>
-      <c r="CH9" s="64"/>
+      <c r="BX9" s="34"/>
+      <c r="BY9" s="34"/>
+      <c r="BZ9" s="34"/>
+      <c r="CA9" s="34"/>
+      <c r="CB9" s="34"/>
+      <c r="CC9" s="34"/>
+      <c r="CD9" s="34"/>
+      <c r="CE9" s="34"/>
+      <c r="CF9" s="34"/>
+      <c r="CG9" s="35"/>
+      <c r="CH9" s="35"/>
     </row>
     <row r="10" spans="1:86" ht="12.2" customHeight="1" thickBot="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="34" t="s">
+      <c r="A10" s="67"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="33"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="33"/>
-      <c r="W10" s="32"/>
-      <c r="X10" s="33"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="33"/>
-      <c r="AA10" s="34"/>
-      <c r="AB10" s="82"/>
-      <c r="AD10" s="25"/>
-      <c r="AE10" s="27"/>
-      <c r="AF10" s="34" t="s">
+      <c r="D10" s="70"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="72"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="72"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="72"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="72"/>
+      <c r="U10" s="71"/>
+      <c r="V10" s="72"/>
+      <c r="W10" s="71"/>
+      <c r="X10" s="72"/>
+      <c r="Y10" s="71"/>
+      <c r="Z10" s="72"/>
+      <c r="AA10" s="69"/>
+      <c r="AB10" s="73"/>
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="68"/>
+      <c r="AF10" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="AG10" s="35"/>
-      <c r="AH10" s="32"/>
-      <c r="AI10" s="33"/>
-      <c r="AJ10" s="32"/>
-      <c r="AK10" s="33"/>
-      <c r="AL10" s="32"/>
-      <c r="AM10" s="33"/>
-      <c r="AN10" s="32"/>
-      <c r="AO10" s="33"/>
-      <c r="AP10" s="32"/>
-      <c r="AQ10" s="33"/>
-      <c r="AR10" s="32"/>
-      <c r="AS10" s="33"/>
-      <c r="AT10" s="32"/>
-      <c r="AU10" s="33"/>
-      <c r="AV10" s="32"/>
-      <c r="AW10" s="33"/>
-      <c r="AX10" s="32"/>
-      <c r="AY10" s="33"/>
-      <c r="AZ10" s="32"/>
-      <c r="BA10" s="33"/>
-      <c r="BB10" s="32"/>
-      <c r="BC10" s="33"/>
-      <c r="BD10" s="88"/>
-      <c r="BE10" s="88"/>
+      <c r="AG10" s="70"/>
+      <c r="AH10" s="71"/>
+      <c r="AI10" s="72"/>
+      <c r="AJ10" s="71"/>
+      <c r="AK10" s="72"/>
+      <c r="AL10" s="71"/>
+      <c r="AM10" s="72"/>
+      <c r="AN10" s="71"/>
+      <c r="AO10" s="72"/>
+      <c r="AP10" s="71"/>
+      <c r="AQ10" s="72"/>
+      <c r="AR10" s="71"/>
+      <c r="AS10" s="72"/>
+      <c r="AT10" s="71"/>
+      <c r="AU10" s="72"/>
+      <c r="AV10" s="71"/>
+      <c r="AW10" s="72"/>
+      <c r="AX10" s="71"/>
+      <c r="AY10" s="72"/>
+      <c r="AZ10" s="71"/>
+      <c r="BA10" s="72"/>
+      <c r="BB10" s="71"/>
+      <c r="BC10" s="72"/>
+      <c r="BD10" s="74"/>
+      <c r="BE10" s="74"/>
     </row>
     <row r="11" spans="1:86" ht="9.75" customHeight="1" thickTop="1">
-      <c r="BG11" s="89" t="s">
+      <c r="BG11" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="BH11" s="89"/>
-      <c r="BI11" s="7"/>
-      <c r="BJ11" s="7"/>
-      <c r="BK11" s="7"/>
-      <c r="BL11" s="7"/>
-      <c r="BM11" s="7"/>
-      <c r="BN11" s="7"/>
-      <c r="BO11" s="69"/>
-      <c r="BP11" s="69"/>
-      <c r="BQ11" s="69"/>
-      <c r="BR11" s="69"/>
-      <c r="BS11" s="69"/>
-      <c r="BT11" s="90"/>
-      <c r="BU11" s="70"/>
-      <c r="BV11" s="71"/>
-      <c r="BW11" s="70"/>
-      <c r="BX11" s="71"/>
-      <c r="BY11" s="70"/>
-      <c r="BZ11" s="71"/>
-      <c r="CA11" s="70"/>
-      <c r="CB11" s="71"/>
-      <c r="CC11" s="70"/>
-      <c r="CD11" s="71"/>
-      <c r="CE11" s="73"/>
-      <c r="CF11" s="74"/>
-      <c r="CG11" s="70"/>
-      <c r="CH11" s="72"/>
+      <c r="BH11" s="75"/>
+      <c r="BI11" s="76"/>
+      <c r="BJ11" s="76"/>
+      <c r="BK11" s="76"/>
+      <c r="BL11" s="76"/>
+      <c r="BM11" s="76"/>
+      <c r="BN11" s="76"/>
+      <c r="BO11" s="77"/>
+      <c r="BP11" s="77"/>
+      <c r="BQ11" s="77"/>
+      <c r="BR11" s="77"/>
+      <c r="BS11" s="77"/>
+      <c r="BT11" s="78"/>
+      <c r="BU11" s="79"/>
+      <c r="BV11" s="80"/>
+      <c r="BW11" s="79"/>
+      <c r="BX11" s="80"/>
+      <c r="BY11" s="79"/>
+      <c r="BZ11" s="80"/>
+      <c r="CA11" s="79"/>
+      <c r="CB11" s="80"/>
+      <c r="CC11" s="79"/>
+      <c r="CD11" s="80"/>
+      <c r="CE11" s="81"/>
+      <c r="CF11" s="82"/>
+      <c r="CG11" s="79"/>
+      <c r="CH11" s="83"/>
     </row>
     <row r="12" spans="1:86" ht="9.75" customHeight="1">
-      <c r="BG12" s="65"/>
-      <c r="BH12" s="65"/>
-      <c r="BI12" s="8"/>
-      <c r="BJ12" s="8"/>
-      <c r="BK12" s="8"/>
-      <c r="BL12" s="8"/>
-      <c r="BM12" s="8"/>
-      <c r="BN12" s="8"/>
-      <c r="BO12" s="66"/>
-      <c r="BP12" s="66"/>
-      <c r="BQ12" s="66"/>
-      <c r="BR12" s="66"/>
-      <c r="BS12" s="66"/>
-      <c r="BT12" s="67"/>
-      <c r="BU12" s="68"/>
-      <c r="BV12" s="67"/>
-      <c r="BW12" s="68"/>
-      <c r="BX12" s="67"/>
-      <c r="BY12" s="68"/>
-      <c r="BZ12" s="67"/>
-      <c r="CA12" s="85"/>
-      <c r="CB12" s="86"/>
-      <c r="CC12" s="68"/>
-      <c r="CD12" s="67"/>
-      <c r="CE12" s="87"/>
-      <c r="CF12" s="86"/>
-      <c r="CG12" s="68"/>
-      <c r="CH12" s="66"/>
+      <c r="BG12" s="84"/>
+      <c r="BH12" s="84"/>
+      <c r="BI12" s="85"/>
+      <c r="BJ12" s="85"/>
+      <c r="BK12" s="85"/>
+      <c r="BL12" s="85"/>
+      <c r="BM12" s="85"/>
+      <c r="BN12" s="85"/>
+      <c r="BO12" s="86"/>
+      <c r="BP12" s="86"/>
+      <c r="BQ12" s="86"/>
+      <c r="BR12" s="86"/>
+      <c r="BS12" s="86"/>
+      <c r="BT12" s="87"/>
+      <c r="BU12" s="88"/>
+      <c r="BV12" s="87"/>
+      <c r="BW12" s="88"/>
+      <c r="BX12" s="87"/>
+      <c r="BY12" s="88"/>
+      <c r="BZ12" s="87"/>
+      <c r="CA12" s="89"/>
+      <c r="CB12" s="90"/>
+      <c r="CC12" s="88"/>
+      <c r="CD12" s="87"/>
+      <c r="CE12" s="91"/>
+      <c r="CF12" s="90"/>
+      <c r="CG12" s="88"/>
+      <c r="CH12" s="86"/>
     </row>
     <row r="14" spans="1:86" ht="9.75" customHeight="1">
-      <c r="BG14" s="54"/>
-      <c r="BH14" s="55"/>
+      <c r="BG14" s="25"/>
+      <c r="BH14" s="26"/>
     </row>
     <row r="15" spans="1:86" ht="11.45" customHeight="1">
-      <c r="BG15" s="56"/>
-      <c r="BH15" s="57"/>
+      <c r="BG15" s="27"/>
+      <c r="BH15" s="28"/>
     </row>
     <row r="16" spans="1:86" ht="11.45" customHeight="1">
-      <c r="BG16" s="58"/>
-      <c r="BH16" s="59"/>
+      <c r="BG16" s="29"/>
+      <c r="BH16" s="30"/>
     </row>
     <row r="17" spans="59:60" ht="11.45" customHeight="1">
-      <c r="BG17" s="60"/>
-      <c r="BH17" s="61"/>
+      <c r="BG17" s="31"/>
+      <c r="BH17" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="223">
-    <mergeCell ref="AJ7:AK7"/>
     <mergeCell ref="CA12:CB12"/>
     <mergeCell ref="CC12:CD12"/>
     <mergeCell ref="CE12:CF12"/>
@@ -2101,12 +2122,6 @@
     <mergeCell ref="BQ11:BR11"/>
     <mergeCell ref="BS11:BT11"/>
     <mergeCell ref="BU11:BV11"/>
-    <mergeCell ref="AN9:AO9"/>
-    <mergeCell ref="AP9:AQ9"/>
-    <mergeCell ref="AR9:AS9"/>
-    <mergeCell ref="AT9:AU9"/>
-    <mergeCell ref="AV9:AW9"/>
-    <mergeCell ref="AX9:AY9"/>
     <mergeCell ref="AZ9:BA9"/>
     <mergeCell ref="BB9:BC9"/>
     <mergeCell ref="BD9:BE9"/>
@@ -2123,6 +2138,12 @@
     <mergeCell ref="AH10:AI10"/>
     <mergeCell ref="AJ10:AK10"/>
     <mergeCell ref="AL10:AM10"/>
+    <mergeCell ref="AN9:AO9"/>
+    <mergeCell ref="AP9:AQ9"/>
+    <mergeCell ref="AR9:AS9"/>
+    <mergeCell ref="AT9:AU9"/>
+    <mergeCell ref="AV9:AW9"/>
+    <mergeCell ref="AX9:AY9"/>
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="U10:V10"/>
     <mergeCell ref="W9:X9"/>
@@ -2170,6 +2191,7 @@
     <mergeCell ref="BD4:BE4"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AJ7:AK7"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="O4:P4"/>

</xml_diff>